<commit_message>
trying to save fig
</commit_message>
<xml_diff>
--- a/franchise_worth.xlsx
+++ b/franchise_worth.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tynka/WizualizacjaDanych/Pokemon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5E20AFE-2593-9F4F-B3AE-5577C7592920}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1734825-A4BE-3F40-A619-59E9D0130264}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14980" yWindow="920" windowWidth="14960" windowHeight="17240" xr2:uid="{84B550E1-7FC6-5744-A56B-F6AD70D304AB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="74">
   <si>
     <t>Pokémon</t>
   </si>
@@ -255,6 +255,9 @@
   </si>
   <si>
     <t>Cartoon character</t>
+  </si>
+  <si>
+    <t>id</t>
   </si>
 </sst>
 </file>
@@ -644,10 +647,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CCBF570-828C-714E-90BF-3A69BE360166}">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -658,403 +661,463 @@
     <col min="6" max="6" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>8</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>10</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>11</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>1996</v>
       </c>
-      <c r="C2" s="2">
+      <c r="D2" s="2">
         <v>115000000000</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>1</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>2</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>1928</v>
       </c>
-      <c r="C3" s="3">
+      <c r="D3" s="3">
         <v>61200000000</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>4</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>48</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="B4">
+      <c r="C4">
         <v>1924</v>
       </c>
-      <c r="C4" s="3">
+      <c r="D4" s="3">
         <v>50200000000</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>44</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>49</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
         <v>13</v>
       </c>
-      <c r="B5">
+      <c r="C5">
         <v>1977</v>
       </c>
-      <c r="C5" s="2">
+      <c r="D5" s="2">
         <v>46700000000</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>14</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>15</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
         <v>16</v>
       </c>
-      <c r="B6">
+      <c r="C6">
         <v>2000</v>
       </c>
-      <c r="C6" s="2">
+      <c r="D6" s="2">
         <v>45400000000</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>17</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>18</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
         <v>19</v>
       </c>
-      <c r="B7">
+      <c r="C7">
         <v>1973</v>
       </c>
-      <c r="C7" s="2">
+      <c r="D7" s="2">
         <v>38300000000</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>20</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>21</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
         <v>22</v>
       </c>
-      <c r="B8">
+      <c r="C8">
         <v>1987</v>
       </c>
-      <c r="C8" s="2">
+      <c r="D8" s="2">
         <v>36300000000</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>23</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>24</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
         <v>26</v>
       </c>
-      <c r="B9">
+      <c r="C9">
         <v>2008</v>
       </c>
-      <c r="C9" s="2">
+      <c r="D9" s="2">
         <v>35200000000</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
         <v>47</v>
       </c>
-      <c r="B10">
+      <c r="C10">
         <v>1997</v>
       </c>
-      <c r="C10" s="2">
+      <c r="D10" s="2">
         <v>34700000000</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>27</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>28</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
         <v>29</v>
       </c>
-      <c r="B11">
+      <c r="C11">
         <v>1974</v>
       </c>
-      <c r="C11" s="2">
+      <c r="D11" s="2">
         <v>33500000000</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>72</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>55</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
         <v>31</v>
       </c>
-      <c r="B12">
+      <c r="C12">
         <v>2003</v>
       </c>
-      <c r="C12" s="3">
+      <c r="D12" s="3">
         <v>31000000000</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>1</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>32</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
         <v>33</v>
       </c>
-      <c r="B13">
+      <c r="C13">
         <v>1939</v>
       </c>
-      <c r="C13" s="3">
+      <c r="D13" s="3">
         <v>29900000000</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>34</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>56</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
         <v>35</v>
       </c>
-      <c r="B14">
+      <c r="C14">
         <v>1962</v>
       </c>
-      <c r="C14" s="3">
+      <c r="D14" s="3">
         <v>36800000000</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>34</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>60</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
         <v>36</v>
       </c>
-      <c r="B15">
+      <c r="C15">
         <v>1984</v>
       </c>
-      <c r="C15" s="3">
+      <c r="D15" s="3">
         <v>25000000000</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>37</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>61</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
         <v>53</v>
       </c>
-      <c r="B16">
+      <c r="C16">
         <v>2005</v>
       </c>
-      <c r="C16" s="3">
+      <c r="D16" s="3">
         <v>22000000000</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>1</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>38</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
         <v>39</v>
       </c>
-      <c r="B17">
+      <c r="C17">
         <v>2006</v>
       </c>
-      <c r="C17" s="3">
+      <c r="D17" s="3">
         <v>21500000000</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>40</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>64</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
         <v>41</v>
       </c>
-      <c r="B18">
+      <c r="C18">
         <v>2012</v>
       </c>
-      <c r="C18">
+      <c r="D18">
         <v>20000000000</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>1</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>42</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
         <v>66</v>
       </c>
-      <c r="B19">
+      <c r="C19">
         <v>1930</v>
       </c>
-      <c r="C19">
+      <c r="D19">
         <v>17460000000</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>4</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>67</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
         <v>69</v>
       </c>
-      <c r="B20">
+      <c r="C20">
         <v>1984</v>
       </c>
-      <c r="C20">
+      <c r="D20">
         <v>17400000000</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>34</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>70</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G20" t="s">
         <v>71</v>
       </c>
     </row>

</xml_diff>